<commit_message>
CustomersWishList Update once more
</commit_message>
<xml_diff>
--- a/CustomersWishList.xlsx
+++ b/CustomersWishList.xlsx
@@ -22,7 +22,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="11">
+  <si>
+    <t xml:space="preserve">currentList</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newList</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bestPrices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">totalCost</t>
+  </si>
   <si>
     <t xml:space="preserve">Milk</t>
   </si>
@@ -34,15 +46,6 @@
   </si>
   <si>
     <t xml:space="preserve">Hennessy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">newList</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prices</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total Cost</t>
   </si>
   <si>
     <t xml:space="preserve">Toothpaste</t>
@@ -156,53 +159,60 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="C1" s="0" t="s">
         <v>1</v>
       </c>
-    </row>
+      <c r="E1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -219,41 +229,56 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -270,39 +295,56 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="0" t="s">
         <v>3</v>
       </c>
     </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>